<commit_message>
Attempting to replicate bug on UPPMAX, this runs fine locally
</commit_message>
<xml_diff>
--- a/R_output_files/Tables/Clusters.xlsx
+++ b/R_output_files/Tables/Clusters.xlsx
@@ -383,14 +383,10 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Mus musculus: Cellular response to chemical stress
-Mus musculus: Neutrophil degranulation
-protein autophosphorylation
-ubiquitin-like protein ligase binding
-cell-cell junction
-cell growth
-positive regulation of kinase activity
-spindle</t>
+          <t>Coronavirus disease - COVID-19 - Mus musculus (house mouse)
+Mus musculus: Cellular responses to stress
+Mus musculus: Intracellular signaling by second messengers
+Mus musculus: Cellular response to chemical stress</t>
         </is>
       </c>
     </row>
@@ -403,13 +399,11 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Non-alcoholic fatty liver disease - Mus musculus (house mouse)
+          <t>Oxidative phosphorylation - Mus musculus (house mouse)
+Non-alcoholic fatty liver disease - Mus musculus (house mouse)
+Mus musculus: Cellular responses to stress
 Mus musculus: Cellular response to chemical stress
-Mus musculus: Neutrophil degranulation
-Mus musculus: Signaling by Receptor Tyrosine Kinases
-response to wounding
-cell growth
-synapse organization</t>
+Mus musculus: Signaling by Receptor Tyrosine Kinases</t>
         </is>
       </c>
     </row>
@@ -422,13 +416,9 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Mus musculus: Neutrophil degranulation
-nucleoside-triphosphatase regulator activity
-mRNA processing
-cellular response to transforming growth factor beta stimulus
-spindle
-positive regulation of kinase activity
-postsynaptic specialization</t>
+          <t>Coronavirus disease - COVID-19 - Mus musculus (house mouse)
+Mus musculus: L13a-mediated translational silencing of Ceruloplasmin expression
+Mus musculus: Cellular responses to stress</t>
         </is>
       </c>
     </row>
@@ -441,14 +431,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Mus musculus: Signaling by Receptor Tyrosine Kinases
-Mus musculus: Cellular response to chemical stress
-postsynaptic specialization
-synapse organization
-muscle tissue development
-response to hypoxia
-embryonic organ development
-ubiquitin-like protein ligase binding</t>
+          <t>Coronavirus disease - COVID-19 - Mus musculus (house mouse)
+Mus musculus: Cellular responses to stress
+Mus musculus: L13a-mediated translational silencing of Ceruloplasmin expression
+Mus musculus: Intracellular signaling by second messengers
+Mus musculus: Signaling by Receptor Tyrosine Kinases
+Mus musculus: Cellular response to chemical stress</t>
         </is>
       </c>
     </row>
@@ -461,21 +449,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Mus musculus: Signaling by Receptor Tyrosine Kinases
-skeletal system development
-positive regulation of kinase activity
-establishment or maintenance of cell polarity
-cell growth
-positive regulation of cell cycle
-regulation of developmental growth
-synapse organization
-muscle tissue development
-response to wounding
-embryonic organ development
-cell-cell junction
-response to hypoxia
-ubiquitin-like protein ligase binding
-cellular response to transforming growth factor beta stimulus</t>
+          <t>Mus musculus: Signaling by Receptor Tyrosine Kinases</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Given up on UPPMAX and running with GO terms. Analysis limited to KEGG and Reactome so it can be run locally.
</commit_message>
<xml_diff>
--- a/R_output_files/Tables/Clusters.xlsx
+++ b/R_output_files/Tables/Clusters.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -422,37 +422,6 @@
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>-0.2259954208058162</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Coronavirus disease - COVID-19 - Mus musculus (house mouse)
-Mus musculus: Cellular responses to stress
-Mus musculus: L13a-mediated translational silencing of Ceruloplasmin expression
-Mus musculus: Intracellular signaling by second messengers
-Mus musculus: Signaling by Receptor Tyrosine Kinases
-Mus musculus: Cellular response to chemical stress</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>-0.1164777958681935</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Mus musculus: Signaling by Receptor Tyrosine Kinases</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>